<commit_message>
Update Tracking Use Case - Robust Analisis & Sequence Diagram (Module GLIK) ver 1.0.xlsx
</commit_message>
<xml_diff>
--- a/Robust Analisis - Likuidasi/Tracking Use Case - Robust Analisis & Sequence Diagram (Module GLIK) ver 1.0.xlsx
+++ b/Robust Analisis - Likuidasi/Tracking Use Case - Robust Analisis & Sequence Diagram (Module GLIK) ver 1.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\Documents\GitHub\GLIK-DM\Robust Analisis - Likuidasi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dimas\Downloads\LPS GLIK\GLIK-DM\Robust Analisis - Likuidasi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1CB5A7-BB83-4101-822E-CDEF16C3F650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B978FD2E-60BF-4D8C-9FE2-F764B0A284C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{9D093FFE-4593-44B8-843D-58E930F801B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{9D093FFE-4593-44B8-843D-58E930F801B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Persiapan (ver 1.0)" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="382">
   <si>
     <t>Nama Use Case</t>
   </si>
@@ -1191,7 +1191,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1834,26 +1834,26 @@
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="2.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="5" style="46" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="8.984375E-2" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.36328125" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="0.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="5" style="25" customWidth="1"/>
-    <col min="11" max="11" width="6.453125" style="25" customWidth="1"/>
-    <col min="12" max="12" width="7.54296875" customWidth="1"/>
-    <col min="13" max="13" width="13.1796875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.08984375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.90625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="15.453125" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" style="25" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="39" t="s">
         <v>3</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="14.5" customHeight="1">
+    <row r="3" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41">
         <v>1</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="41">
         <v>2</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="41">
         <v>3</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="6" spans="2:16">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="41">
         <v>4</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="7" spans="2:16">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="41">
         <v>5</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="41">
         <v>6</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="41">
         <v>7</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="41">
         <v>8</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="41">
         <v>9</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="41">
         <v>10</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="41">
         <v>11</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="41">
         <v>12</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="41">
         <v>13</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="41">
         <v>14</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="17" spans="2:16">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="41">
         <v>15</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="18" spans="2:16">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="41">
         <v>16</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="19" spans="2:16">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="24"/>
       <c r="C19" s="7"/>
       <c r="D19" s="11"/>
@@ -2606,7 +2606,7 @@
       <c r="J19" s="38"/>
       <c r="K19" s="35"/>
     </row>
-    <row r="20" spans="2:16">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="24"/>
       <c r="C20" s="7"/>
       <c r="D20" s="11"/>
@@ -2618,7 +2618,7 @@
       <c r="J20" s="38"/>
       <c r="K20" s="35"/>
     </row>
-    <row r="21" spans="2:16">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="24"/>
       <c r="C21" s="7"/>
       <c r="D21" s="11"/>
@@ -2644,30 +2644,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B26C05-1418-48A4-9E35-BE8C2DB41FAB}">
   <dimension ref="B2:P67"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="2.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6328125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="6" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.90625" customWidth="1"/>
-    <col min="12" max="12" width="6.6328125" customWidth="1"/>
-    <col min="13" max="13" width="13.453125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="14" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7265625" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="16" customHeight="1">
+    <row r="3" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
         <v>1</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="8">
         <v>3</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="6" spans="2:16">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
         <v>4</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="7" spans="2:16">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
         <v>5</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
         <v>6</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
         <v>7</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
         <v>8</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="8">
         <v>9</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="8">
         <v>10</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="8">
         <v>11</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="8">
         <v>12</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="8">
         <v>13</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="8">
         <v>14</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="17" spans="2:16">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
         <v>15</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="18" spans="2:16">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <v>16</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="19" spans="2:16">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
         <v>17</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="2:16">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
         <v>18</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="21" spans="2:16">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="8">
         <v>19</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="22" spans="2:16">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
         <v>20</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="2:16">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="8">
         <v>21</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="24" spans="2:16">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="8">
         <v>22</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="25" spans="2:16">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="8">
         <v>23</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="26" spans="2:16">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="8">
         <v>24</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="27" spans="2:16">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="8">
         <v>25</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="28" spans="2:16">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="8">
         <v>26</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="29" spans="2:16">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="8">
         <v>27</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="2:16">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="8">
         <v>28</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="31" spans="2:16">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="8">
         <v>29</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="32" spans="2:16">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="8">
         <v>30</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="33" spans="2:16">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="8">
         <v>31</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="34" spans="2:16">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="8">
         <v>32</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="35" spans="2:16">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="8">
         <v>33</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="36" spans="2:16">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="8">
         <v>34</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="37" spans="2:16">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="8">
         <v>35</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="38" spans="2:16">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="8">
         <v>36</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="39" spans="2:16">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="8">
         <v>37</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="40" spans="2:16">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="8">
         <v>38</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="41" spans="2:16">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="8">
         <v>39</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="42" spans="2:16">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="8">
         <v>40</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="43" spans="2:16">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="8">
         <v>41</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="44" spans="2:16">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="8">
         <v>42</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="45" spans="2:16">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" s="8">
         <v>43</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="46" spans="2:16" ht="14" customHeight="1">
+    <row r="46" spans="2:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="8">
         <v>44</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="47" spans="2:16" ht="14.5" customHeight="1">
+    <row r="47" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="8">
         <v>45</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="48" spans="2:16">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="8">
         <v>46</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="49" spans="2:16">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" s="8">
         <v>47</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="50" spans="2:16">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="8">
         <v>48</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="51" spans="2:16">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="8">
         <v>49</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="52" spans="2:16">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="8">
         <v>50</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="53" spans="2:16">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="8">
         <v>51</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="54" spans="2:16">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="8">
         <v>52</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="55" spans="2:16">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B55" s="8">
         <v>53</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="56" spans="2:16">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B56" s="8">
         <v>54</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="57" spans="2:16">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B57" s="8">
         <v>55</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="58" spans="2:16">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B58" s="8">
         <v>56</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="59" spans="2:16">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B59" s="8">
         <v>57</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="60" spans="2:16">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B60" s="8">
         <v>58</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="61" spans="2:16">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B61" s="8">
         <v>59</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="62" spans="2:16">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B62" s="8">
         <v>60</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="63" spans="2:16">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B63" s="8">
         <v>61</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="64" spans="2:16">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B64" s="8">
         <v>62</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="65" spans="2:16">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B65" s="8">
         <v>63</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="66" spans="2:16">
+    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B66" s="8">
         <v>64</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="67" spans="2:16">
+    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B67" s="8">
         <v>65</v>
       </c>
@@ -5661,29 +5661,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F6D62D-E7AF-48B8-BDB9-AC8C4457F551}">
   <dimension ref="B2:P30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="2.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="4.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7265625" customWidth="1"/>
-    <col min="11" max="11" width="7.26953125" customWidth="1"/>
-    <col min="12" max="12" width="6.54296875" customWidth="1"/>
-    <col min="13" max="14" width="13.1796875" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.90625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="15.36328125" customWidth="1"/>
+    <col min="2" max="2" width="2.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" customWidth="1"/>
+    <col min="13" max="14" width="13.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="14.5" customHeight="1">
+    <row r="3" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
         <v>1</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="8">
         <v>3</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="6" spans="2:16">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
         <v>4</v>
       </c>
@@ -5912,7 +5912,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="15" customHeight="1">
+    <row r="7" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
         <v>5</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
         <v>6</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
         <v>7</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
         <v>8</v>
       </c>
@@ -6092,7 +6092,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="8">
         <v>9</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="8">
         <v>10</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="8">
         <v>11</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="8">
         <v>12</v>
       </c>
@@ -6274,7 +6274,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="8">
         <v>13</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="8">
         <v>14</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="17" spans="2:16">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
         <v>15</v>
       </c>
@@ -6409,7 +6409,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="18" spans="2:16">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <v>16</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="19" spans="2:16">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
         <v>17</v>
       </c>
@@ -6499,7 +6499,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="2:16">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
         <v>18</v>
       </c>
@@ -6544,7 +6544,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="21" spans="2:16">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="8">
         <v>19</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="22" spans="2:16">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
         <v>20</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="2:16">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="8">
         <v>21</v>
       </c>
@@ -6681,7 +6681,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="24" spans="2:16">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="8">
         <v>22</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="25" spans="2:16">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="8">
         <v>23</v>
       </c>
@@ -6771,7 +6771,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="26" spans="2:16">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="8">
         <v>24</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="27" spans="2:16">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="8">
         <v>25</v>
       </c>
@@ -6861,7 +6861,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="28" spans="2:16">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="8">
         <v>26</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="29" spans="2:16">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="8">
         <v>27</v>
       </c>
@@ -6951,7 +6951,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="2:16">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="8">
         <v>28</v>
       </c>
@@ -7012,28 +7012,28 @@
   <dimension ref="B2:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K7" sqref="K7:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="2.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6328125" style="25" customWidth="1"/>
-    <col min="11" max="11" width="6.26953125" customWidth="1"/>
-    <col min="12" max="12" width="7.1796875" customWidth="1"/>
-    <col min="13" max="14" width="13.1796875" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.90625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="15.36328125" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="25" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" customWidth="1"/>
+    <col min="13" max="14" width="13.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="3" spans="2:16">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="26">
         <v>1</v>
       </c>
@@ -7103,9 +7103,11 @@
         <v>371</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K3" s="12"/>
+        <v>374</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L3" s="34" t="s">
         <v>373</v>
       </c>
@@ -7122,7 +7124,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="26">
         <v>2</v>
       </c>
@@ -7143,9 +7145,11 @@
         <v>371</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K4" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L4" s="34" t="s">
         <v>373</v>
       </c>
@@ -7162,7 +7166,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="26">
         <v>3</v>
       </c>
@@ -7183,9 +7187,11 @@
         <v>371</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K5" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L5" s="34" t="s">
         <v>373</v>
       </c>
@@ -7202,7 +7208,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="6" spans="2:16">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="26">
         <v>4</v>
       </c>
@@ -7223,9 +7229,11 @@
         <v>371</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K6" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L6" s="34" t="s">
         <v>373</v>
       </c>
@@ -7242,7 +7250,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="7" spans="2:16">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="26">
         <v>5</v>
       </c>
@@ -7263,9 +7271,11 @@
         <v>371</v>
       </c>
       <c r="J7" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K7" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L7" s="34" t="s">
         <v>373</v>
       </c>
@@ -7282,7 +7292,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="26">
         <v>6</v>
       </c>
@@ -7303,9 +7313,11 @@
         <v>371</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K8" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L8" s="34" t="s">
         <v>373</v>
       </c>
@@ -7322,7 +7334,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="26">
         <v>7</v>
       </c>
@@ -7345,9 +7357,11 @@
         <v>371</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K9" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L9" s="34" t="s">
         <v>373</v>
       </c>
@@ -7364,7 +7378,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="26">
         <v>8</v>
       </c>
@@ -7406,7 +7420,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="26">
         <v>9</v>
       </c>
@@ -7448,7 +7462,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="26">
         <v>10</v>
       </c>
@@ -7469,9 +7483,11 @@
         <v>371</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K12" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L12" s="34" t="s">
         <v>373</v>
       </c>
@@ -7488,7 +7504,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="26">
         <v>11</v>
       </c>
@@ -7509,9 +7525,11 @@
         <v>371</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K13" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L13" s="34" t="s">
         <v>373</v>
       </c>
@@ -7528,7 +7546,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="26">
         <v>12</v>
       </c>
@@ -7549,9 +7567,11 @@
         <v>371</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K14" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L14" s="34" t="s">
         <v>373</v>
       </c>
@@ -7568,7 +7588,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="26">
         <v>13</v>
       </c>
@@ -7589,9 +7609,11 @@
         <v>371</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K15" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L15" s="34" t="s">
         <v>373</v>
       </c>
@@ -7608,7 +7630,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="26">
         <v>14</v>
       </c>
@@ -7629,9 +7651,11 @@
         <v>371</v>
       </c>
       <c r="J16" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K16" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L16" s="34" t="s">
         <v>373</v>
       </c>
@@ -7648,7 +7672,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="17" spans="2:16">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="26">
         <v>15</v>
       </c>
@@ -7669,9 +7693,11 @@
         <v>371</v>
       </c>
       <c r="J17" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="K17" s="31"/>
+        <v>374</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="L17" s="34" t="s">
         <v>373</v>
       </c>
@@ -7704,19 +7730,19 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="31"/>
-    <col min="2" max="2" width="2.1796875" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="31"/>
-    <col min="4" max="4" width="13.453125" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" style="31" customWidth="1"/>
-    <col min="7" max="7" width="67.08984375" style="31" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="31"/>
+    <col min="1" max="1" width="8.7109375" style="31"/>
+    <col min="2" max="2" width="2.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="31"/>
+    <col min="4" max="4" width="13.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="31" customWidth="1"/>
+    <col min="7" max="7" width="67.140625" style="31" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="31"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="14.5" customHeight="1">
+    <row r="2" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="70" t="s">
         <v>350</v>
       </c>
@@ -7726,7 +7752,7 @@
       <c r="F2" s="70"/>
       <c r="G2" s="70"/>
     </row>
-    <row r="3" spans="2:7" s="48" customFormat="1" ht="14.5" customHeight="1">
+    <row r="3" spans="2:7" s="48" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="49" t="s">
         <v>3</v>
       </c>
@@ -7746,7 +7772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="14.5" customHeight="1">
+    <row r="4" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="71">
         <v>1</v>
       </c>
@@ -7767,7 +7793,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="14.5" customHeight="1">
+    <row r="5" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="71"/>
       <c r="C5" s="72"/>
       <c r="D5" s="51" t="s">
@@ -7779,7 +7805,7 @@
       <c r="F5" s="71"/>
       <c r="G5" s="72"/>
     </row>
-    <row r="6" spans="2:7" ht="14.5" customHeight="1">
+    <row r="6" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="71"/>
       <c r="C6" s="72"/>
       <c r="D6" s="51" t="s">
@@ -7791,7 +7817,7 @@
       <c r="F6" s="71"/>
       <c r="G6" s="72"/>
     </row>
-    <row r="7" spans="2:7" ht="14.5" customHeight="1">
+    <row r="7" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="71"/>
       <c r="C7" s="72"/>
       <c r="D7" s="51" t="s">
@@ -7803,7 +7829,7 @@
       <c r="F7" s="71"/>
       <c r="G7" s="72"/>
     </row>
-    <row r="8" spans="2:7" ht="14.5" customHeight="1">
+    <row r="8" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="52">
         <v>2</v>
       </c>
@@ -7823,7 +7849,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="14.5" customHeight="1">
+    <row r="11" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="70" t="s">
         <v>351</v>
       </c>
@@ -7833,7 +7859,7 @@
       <c r="F11" s="70"/>
       <c r="G11" s="70"/>
     </row>
-    <row r="12" spans="2:7" ht="14.5" customHeight="1">
+    <row r="12" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="49" t="s">
         <v>3</v>
       </c>
@@ -7853,7 +7879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="14.5" customHeight="1">
+    <row r="13" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="71">
         <v>1</v>
       </c>
@@ -7874,7 +7900,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="14.5" customHeight="1">
+    <row r="14" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="71"/>
       <c r="C14" s="72"/>
       <c r="D14" s="51" t="s">
@@ -7886,7 +7912,7 @@
       <c r="F14" s="71"/>
       <c r="G14" s="72"/>
     </row>
-    <row r="15" spans="2:7" ht="14.5" customHeight="1">
+    <row r="15" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="71"/>
       <c r="C15" s="72"/>
       <c r="D15" s="51" t="s">
@@ -7898,7 +7924,7 @@
       <c r="F15" s="71"/>
       <c r="G15" s="72"/>
     </row>
-    <row r="16" spans="2:7" ht="14.5" customHeight="1">
+    <row r="16" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="71"/>
       <c r="C16" s="72"/>
       <c r="D16" s="51" t="s">
@@ -7910,7 +7936,7 @@
       <c r="F16" s="71"/>
       <c r="G16" s="72"/>
     </row>
-    <row r="17" spans="2:7" ht="14.5" customHeight="1">
+    <row r="17" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="52">
         <v>2</v>
       </c>
@@ -7930,7 +7956,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="14.5" customHeight="1">
+    <row r="20" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="70" t="s">
         <v>353</v>
       </c>
@@ -7940,7 +7966,7 @@
       <c r="F20" s="70"/>
       <c r="G20" s="70"/>
     </row>
-    <row r="21" spans="2:7" ht="14.5" customHeight="1">
+    <row r="21" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="49" t="s">
         <v>3</v>
       </c>
@@ -7960,7 +7986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="14.5" customHeight="1">
+    <row r="22" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="71">
         <v>1</v>
       </c>
@@ -7981,7 +8007,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="14.5" customHeight="1">
+    <row r="23" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="71"/>
       <c r="C23" s="72"/>
       <c r="D23" s="51" t="s">
@@ -7993,7 +8019,7 @@
       <c r="F23" s="71"/>
       <c r="G23" s="74"/>
     </row>
-    <row r="24" spans="2:7" ht="14.5" customHeight="1">
+    <row r="24" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="71"/>
       <c r="C24" s="72"/>
       <c r="D24" s="51" t="s">
@@ -8005,7 +8031,7 @@
       <c r="F24" s="71"/>
       <c r="G24" s="74"/>
     </row>
-    <row r="25" spans="2:7" ht="14.5" customHeight="1">
+    <row r="25" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="71"/>
       <c r="C25" s="72"/>
       <c r="D25" s="51" t="s">
@@ -8017,7 +8043,7 @@
       <c r="F25" s="71"/>
       <c r="G25" s="74"/>
     </row>
-    <row r="26" spans="2:7" ht="14.5" customHeight="1">
+    <row r="26" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="52">
         <v>2</v>
       </c>

</xml_diff>